<commit_message>
Implement Download Queue Items operation
</commit_message>
<xml_diff>
--- a/Workbooks/EN/Queues.xlsx
+++ b/Workbooks/EN/Queues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26A24BB5-BF96-4E2C-8F2C-71A45A8024F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A260A1F-19D1-44DE-87B5-149DC29B4746}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,8 @@
     <sheet name="Get" sheetId="4" r:id="rId1"/>
     <sheet name="Create" sheetId="1" r:id="rId2"/>
     <sheet name="Delete" sheetId="2" r:id="rId3"/>
+    <sheet name="Download Queue Items" sheetId="5" r:id="rId4"/>
+    <sheet name="Upload Queue Items" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -65,6 +67,18 @@
   </si>
   <si>
     <t>Organization Unit Name</t>
+  </si>
+  <si>
+    <t>結果</t>
+  </si>
+  <si>
+    <t>Queue Items Filepath</t>
+  </si>
+  <si>
+    <t>Commit Type</t>
+  </si>
+  <si>
+    <t>Download Folderpath</t>
   </si>
 </sst>
 </file>
@@ -106,7 +120,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -233,11 +247,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -281,13 +306,24 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="32">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -295,7 +331,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </left>
@@ -308,6 +344,246 @@
         <bottom style="thin">
           <color theme="0" tint="-0.34998626667073579"/>
         </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+        <vertical style="thin">
+          <color theme="5"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="5"/>
+        </horizontal>
       </border>
       <protection locked="1" hidden="0"/>
     </dxf>
@@ -676,6 +952,31 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="solid">
@@ -897,17 +1198,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H201" headerRowDxfId="22" dataDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H201" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{74C6F987-536B-46B5-AFA6-A7F27476553A}" name="Organization Unit ID" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{C8277EF1-3260-4C74-8C12-2B8EFAF635A0}" name="Organization Unit Name" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{22E1BA7C-1596-4556-9F97-A21C0B7470BC}" name="Queue ID" dataDxfId="18"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Queue Name" totalsRowLabel="Total" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Description" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Unique Reference" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{EA8DF354-2F10-4E45-801A-56D5F80552D8}" name="Auto Retry" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Max # of retries" totalsRowFunction="count" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{74C6F987-536B-46B5-AFA6-A7F27476553A}" name="Organization Unit ID" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{C8277EF1-3260-4C74-8C12-2B8EFAF635A0}" name="Organization Unit Name" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{22E1BA7C-1596-4556-9F97-A21C0B7470BC}" name="Queue ID" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Queue Name" totalsRowLabel="Total" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Description" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Unique Reference" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{EA8DF354-2F10-4E45-801A-56D5F80552D8}" name="Auto Retry" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Max # of retries" totalsRowFunction="count" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -917,14 +1218,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H201" totalsRowShown="0">
   <autoFilter ref="A1:H201" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="8" xr3:uid="{A7178589-1B6B-47CF-BAAC-D2F2E4BB9988}" name="Organization Unit Name" dataDxfId="13"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Queue Name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="Unique Reference" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{07A3D78A-00F5-4019-BC61-B83E2CEDEEA5}" name="Auto Retry" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{5CA1824C-85AD-40DB-A0CE-9853C443448E}" name="Max # of retries" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{A7178589-1B6B-47CF-BAAC-D2F2E4BB9988}" name="Organization Unit Name" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Queue Name" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Description" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{4D652F4A-5125-4BA7-BCE0-BCD13A330E29}" name="Unique Reference" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{07A3D78A-00F5-4019-BC61-B83E2CEDEEA5}" name="Auto Retry" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5CA1824C-85AD-40DB-A0CE-9853C443448E}" name="Max # of retries" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="ID" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{D1E6EAA2-70C4-4033-9FEE-92C367F3E3E4}" name="Result" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -934,11 +1235,38 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A1:E201" totalsRowShown="0">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="5" xr3:uid="{FC48162A-FC37-4E8B-A499-5A38EF9C6126}" name="Organization Unit ID" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{5376A05A-37AF-4421-8DB1-36A26B07A3C8}" name="Organization Unit Name" dataDxfId="4"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Queue ID" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Queue Name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{FC48162A-FC37-4E8B-A499-5A38EF9C6126}" name="Organization Unit ID" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{5376A05A-37AF-4421-8DB1-36A26B07A3C8}" name="Organization Unit Name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Queue ID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{77482336-B9C3-42EA-B117-2D0B1D764C3A}" name="Queue Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{9F11D09F-EBB8-481F-9883-602BE1C1BEC7}" name="Result" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{BBB7F12E-D263-4590-BCE2-61D82D618DB1}" name="Table135" displayName="Table135" ref="A1:D201" totalsRowShown="0">
+  <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{A0F02CF9-2422-4237-BCF2-7AC4FEA2A0E5}" name="Organization Unit Name" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{C64A64C1-6175-416D-A899-A6A78F2BCFFD}" name="Queue Name" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{37F9878F-61EF-41DF-82D6-B66A203E99DE}" name="Download Folderpath" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4B37078C-0815-4876-9483-02F0C251D161}" name="Result" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{BCB67D51-E017-4B9D-B6B1-7213CB9837F8}" name="Table1356" displayName="Table1356" ref="A1:E201" totalsRowShown="0">
+  <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="4" xr3:uid="{DA48F80D-A0D8-4817-A87A-D1562C993C3C}" name="Organization Unit Name" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C59AF576-8586-407D-B9AB-05ACA94BF07F}" name="Queue Name" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{E4F8EBBA-8809-4C1B-AE66-772B45052FD0}" name="Queue Items Filepath" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{CD3F8AA2-6168-4A6C-A422-84C3410D9128}" name="Commit Type" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{844BAEE1-D0DF-4267-935C-6B2CC0F525CC}" name="結果" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6769,4 +7097,2692 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E987D8-7C5C-43B6-8BCE-4DEE40D0A7B1}">
+  <dimension ref="A1:D201"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="32"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="32"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="32"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="32"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="32"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="32"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="32"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="32"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="32"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="32"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="32"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="32"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="32"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="32"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="32"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="32"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="32"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="32"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="32"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="32"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="32"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="32"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="32"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="32"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="32"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="32"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="32"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="32"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="32"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="32"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="32"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="32"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="32"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="32"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="32"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="32"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="32"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="32"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="32"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="32"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="32"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="32"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="32"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="32"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="32"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="32"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="32"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="32"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="32"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="32"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="32"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="32"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="32"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="32"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="32"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="32"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="32"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="32"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="32"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="32"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="32"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="32"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="32"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="32"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="32"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="32"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="32"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="32"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="32"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="32"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="32"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="32"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="32"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="32"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="32"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="32"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="32"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="32"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="32"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="32"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="32"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="32"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="32"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="32"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="32"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="32"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="32"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="32"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="32"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="32"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="32"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="32"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="32"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="32"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="32"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="32"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="32"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="32"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="32"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="32"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="32"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="32"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="32"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="32"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="32"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="32"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="32"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="32"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="32"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="32"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="32"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="32"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123" s="27"/>
+      <c r="B123" s="27"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="32"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124" s="27"/>
+      <c r="B124" s="27"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="32"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="32"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126" s="27"/>
+      <c r="B126" s="27"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="32"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127" s="27"/>
+      <c r="B127" s="27"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="32"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128" s="27"/>
+      <c r="B128" s="27"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="32"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129" s="27"/>
+      <c r="B129" s="27"/>
+      <c r="C129" s="28"/>
+      <c r="D129" s="32"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130" s="27"/>
+      <c r="B130" s="27"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="32"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A131" s="27"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="28"/>
+      <c r="D131" s="32"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A132" s="27"/>
+      <c r="B132" s="27"/>
+      <c r="C132" s="28"/>
+      <c r="D132" s="32"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A133" s="27"/>
+      <c r="B133" s="27"/>
+      <c r="C133" s="28"/>
+      <c r="D133" s="32"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A134" s="27"/>
+      <c r="B134" s="27"/>
+      <c r="C134" s="28"/>
+      <c r="D134" s="32"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135" s="27"/>
+      <c r="B135" s="27"/>
+      <c r="C135" s="28"/>
+      <c r="D135" s="32"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136" s="27"/>
+      <c r="B136" s="27"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="32"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A137" s="27"/>
+      <c r="B137" s="27"/>
+      <c r="C137" s="28"/>
+      <c r="D137" s="32"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A138" s="27"/>
+      <c r="B138" s="27"/>
+      <c r="C138" s="28"/>
+      <c r="D138" s="32"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139" s="27"/>
+      <c r="B139" s="27"/>
+      <c r="C139" s="28"/>
+      <c r="D139" s="32"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140" s="27"/>
+      <c r="B140" s="27"/>
+      <c r="C140" s="28"/>
+      <c r="D140" s="32"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141" s="27"/>
+      <c r="B141" s="27"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="32"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A142" s="27"/>
+      <c r="B142" s="27"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="32"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A143" s="27"/>
+      <c r="B143" s="27"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="32"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144" s="27"/>
+      <c r="B144" s="27"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="32"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145" s="27"/>
+      <c r="B145" s="27"/>
+      <c r="C145" s="28"/>
+      <c r="D145" s="32"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146" s="27"/>
+      <c r="B146" s="27"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="32"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147" s="27"/>
+      <c r="B147" s="27"/>
+      <c r="C147" s="28"/>
+      <c r="D147" s="32"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A148" s="27"/>
+      <c r="B148" s="27"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="32"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149" s="27"/>
+      <c r="B149" s="27"/>
+      <c r="C149" s="28"/>
+      <c r="D149" s="32"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150" s="27"/>
+      <c r="B150" s="27"/>
+      <c r="C150" s="28"/>
+      <c r="D150" s="32"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151" s="27"/>
+      <c r="B151" s="27"/>
+      <c r="C151" s="28"/>
+      <c r="D151" s="32"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152" s="27"/>
+      <c r="B152" s="27"/>
+      <c r="C152" s="28"/>
+      <c r="D152" s="32"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153" s="27"/>
+      <c r="B153" s="27"/>
+      <c r="C153" s="28"/>
+      <c r="D153" s="32"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154" s="27"/>
+      <c r="B154" s="27"/>
+      <c r="C154" s="28"/>
+      <c r="D154" s="32"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155" s="27"/>
+      <c r="B155" s="27"/>
+      <c r="C155" s="28"/>
+      <c r="D155" s="32"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156" s="27"/>
+      <c r="B156" s="27"/>
+      <c r="C156" s="28"/>
+      <c r="D156" s="32"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157" s="27"/>
+      <c r="B157" s="27"/>
+      <c r="C157" s="28"/>
+      <c r="D157" s="32"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158" s="27"/>
+      <c r="B158" s="27"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="32"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159" s="27"/>
+      <c r="B159" s="27"/>
+      <c r="C159" s="28"/>
+      <c r="D159" s="32"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160" s="27"/>
+      <c r="B160" s="27"/>
+      <c r="C160" s="28"/>
+      <c r="D160" s="32"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161" s="27"/>
+      <c r="B161" s="27"/>
+      <c r="C161" s="28"/>
+      <c r="D161" s="32"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162" s="27"/>
+      <c r="B162" s="27"/>
+      <c r="C162" s="28"/>
+      <c r="D162" s="32"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163" s="27"/>
+      <c r="B163" s="27"/>
+      <c r="C163" s="28"/>
+      <c r="D163" s="32"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164" s="27"/>
+      <c r="B164" s="27"/>
+      <c r="C164" s="28"/>
+      <c r="D164" s="32"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165" s="27"/>
+      <c r="B165" s="27"/>
+      <c r="C165" s="28"/>
+      <c r="D165" s="32"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A166" s="27"/>
+      <c r="B166" s="27"/>
+      <c r="C166" s="28"/>
+      <c r="D166" s="32"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A167" s="27"/>
+      <c r="B167" s="27"/>
+      <c r="C167" s="28"/>
+      <c r="D167" s="32"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A168" s="27"/>
+      <c r="B168" s="27"/>
+      <c r="C168" s="28"/>
+      <c r="D168" s="32"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169" s="27"/>
+      <c r="B169" s="27"/>
+      <c r="C169" s="28"/>
+      <c r="D169" s="32"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170" s="27"/>
+      <c r="B170" s="27"/>
+      <c r="C170" s="28"/>
+      <c r="D170" s="32"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171" s="27"/>
+      <c r="B171" s="27"/>
+      <c r="C171" s="28"/>
+      <c r="D171" s="32"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172" s="27"/>
+      <c r="B172" s="27"/>
+      <c r="C172" s="28"/>
+      <c r="D172" s="32"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173" s="27"/>
+      <c r="B173" s="27"/>
+      <c r="C173" s="28"/>
+      <c r="D173" s="32"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174" s="27"/>
+      <c r="B174" s="27"/>
+      <c r="C174" s="28"/>
+      <c r="D174" s="32"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175" s="27"/>
+      <c r="B175" s="27"/>
+      <c r="C175" s="28"/>
+      <c r="D175" s="32"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176" s="27"/>
+      <c r="B176" s="27"/>
+      <c r="C176" s="28"/>
+      <c r="D176" s="32"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177" s="27"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="28"/>
+      <c r="D177" s="32"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178" s="27"/>
+      <c r="B178" s="27"/>
+      <c r="C178" s="28"/>
+      <c r="D178" s="32"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179" s="27"/>
+      <c r="B179" s="27"/>
+      <c r="C179" s="28"/>
+      <c r="D179" s="32"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180" s="27"/>
+      <c r="B180" s="27"/>
+      <c r="C180" s="28"/>
+      <c r="D180" s="32"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181" s="27"/>
+      <c r="B181" s="27"/>
+      <c r="C181" s="28"/>
+      <c r="D181" s="32"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182" s="27"/>
+      <c r="B182" s="27"/>
+      <c r="C182" s="28"/>
+      <c r="D182" s="32"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183" s="27"/>
+      <c r="B183" s="27"/>
+      <c r="C183" s="28"/>
+      <c r="D183" s="32"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184" s="27"/>
+      <c r="B184" s="27"/>
+      <c r="C184" s="28"/>
+      <c r="D184" s="32"/>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185" s="27"/>
+      <c r="B185" s="27"/>
+      <c r="C185" s="28"/>
+      <c r="D185" s="32"/>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186" s="27"/>
+      <c r="B186" s="27"/>
+      <c r="C186" s="28"/>
+      <c r="D186" s="32"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187" s="27"/>
+      <c r="B187" s="27"/>
+      <c r="C187" s="28"/>
+      <c r="D187" s="32"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188" s="27"/>
+      <c r="B188" s="27"/>
+      <c r="C188" s="28"/>
+      <c r="D188" s="32"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189" s="27"/>
+      <c r="B189" s="27"/>
+      <c r="C189" s="28"/>
+      <c r="D189" s="32"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190" s="27"/>
+      <c r="B190" s="27"/>
+      <c r="C190" s="28"/>
+      <c r="D190" s="32"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191" s="27"/>
+      <c r="B191" s="27"/>
+      <c r="C191" s="28"/>
+      <c r="D191" s="32"/>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192" s="27"/>
+      <c r="B192" s="27"/>
+      <c r="C192" s="28"/>
+      <c r="D192" s="32"/>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193" s="27"/>
+      <c r="B193" s="27"/>
+      <c r="C193" s="28"/>
+      <c r="D193" s="32"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194" s="27"/>
+      <c r="B194" s="27"/>
+      <c r="C194" s="28"/>
+      <c r="D194" s="32"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195" s="27"/>
+      <c r="B195" s="27"/>
+      <c r="C195" s="28"/>
+      <c r="D195" s="32"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A196" s="27"/>
+      <c r="B196" s="27"/>
+      <c r="C196" s="28"/>
+      <c r="D196" s="32"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A197" s="27"/>
+      <c r="B197" s="27"/>
+      <c r="C197" s="28"/>
+      <c r="D197" s="32"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A198" s="27"/>
+      <c r="B198" s="27"/>
+      <c r="C198" s="28"/>
+      <c r="D198" s="32"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199" s="27"/>
+      <c r="B199" s="27"/>
+      <c r="C199" s="28"/>
+      <c r="D199" s="32"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A200" s="27"/>
+      <c r="B200" s="27"/>
+      <c r="C200" s="28"/>
+      <c r="D200" s="32"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A201" s="33"/>
+      <c r="B201" s="33"/>
+      <c r="C201" s="34"/>
+      <c r="D201" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D578035-D73C-4A6A-820B-64D1D259E97E}">
+  <dimension ref="A1:E201"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.90625" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="29" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="27"/>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="32"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="27"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="27"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="32"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="32"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="27"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="27"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="32"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="27"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="32"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="27"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="27"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="27"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="27"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="27"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="27"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="32"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="32"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="32"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="27"/>
+      <c r="B24" s="27"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="27"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="32"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="27"/>
+      <c r="B26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="32"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="32"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="27"/>
+      <c r="B30" s="27"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="32"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="27"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="32"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="32"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="27"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="32"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="27"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="32"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="27"/>
+      <c r="B35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="32"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="27"/>
+      <c r="B36" s="27"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="32"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="32"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="27"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="32"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
+      <c r="B39" s="27"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="32"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
+      <c r="B40" s="27"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="32"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="32"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="27"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="28"/>
+      <c r="E42" s="32"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" s="27"/>
+      <c r="B43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="32"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" s="27"/>
+      <c r="B44" s="27"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28"/>
+      <c r="E44" s="32"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="27"/>
+      <c r="B45" s="27"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="28"/>
+      <c r="E45" s="32"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="27"/>
+      <c r="B46" s="27"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="32"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="27"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="28"/>
+      <c r="E47" s="32"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="27"/>
+      <c r="B48" s="27"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="32"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="27"/>
+      <c r="B49" s="27"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="32"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="27"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="32"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A51" s="27"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="32"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="32"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="32"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="27"/>
+      <c r="B54" s="27"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="32"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A55" s="27"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="32"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A56" s="27"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="28"/>
+      <c r="E56" s="32"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A57" s="27"/>
+      <c r="B57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="32"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A58" s="27"/>
+      <c r="B58" s="27"/>
+      <c r="C58" s="28"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="32"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A59" s="27"/>
+      <c r="B59" s="27"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="28"/>
+      <c r="E59" s="32"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A60" s="27"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="28"/>
+      <c r="E60" s="32"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A61" s="27"/>
+      <c r="B61" s="27"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="32"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A62" s="27"/>
+      <c r="B62" s="27"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="32"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A63" s="27"/>
+      <c r="B63" s="27"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="28"/>
+      <c r="E63" s="32"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A64" s="27"/>
+      <c r="B64" s="27"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="32"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="27"/>
+      <c r="B65" s="27"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="28"/>
+      <c r="E65" s="32"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="27"/>
+      <c r="B66" s="27"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="28"/>
+      <c r="E66" s="32"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="27"/>
+      <c r="B67" s="27"/>
+      <c r="C67" s="28"/>
+      <c r="D67" s="28"/>
+      <c r="E67" s="32"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="27"/>
+      <c r="B68" s="27"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="28"/>
+      <c r="E68" s="32"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="27"/>
+      <c r="B69" s="27"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="32"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="27"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+      <c r="E70" s="32"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="27"/>
+      <c r="B71" s="27"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="32"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="27"/>
+      <c r="B72" s="27"/>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+      <c r="E72" s="32"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="27"/>
+      <c r="B73" s="27"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="32"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="27"/>
+      <c r="B74" s="27"/>
+      <c r="C74" s="28"/>
+      <c r="D74" s="28"/>
+      <c r="E74" s="32"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="27"/>
+      <c r="B75" s="27"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="32"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="27"/>
+      <c r="B76" s="27"/>
+      <c r="C76" s="28"/>
+      <c r="D76" s="28"/>
+      <c r="E76" s="32"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="27"/>
+      <c r="B77" s="27"/>
+      <c r="C77" s="28"/>
+      <c r="D77" s="28"/>
+      <c r="E77" s="32"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="27"/>
+      <c r="B78" s="27"/>
+      <c r="C78" s="28"/>
+      <c r="D78" s="28"/>
+      <c r="E78" s="32"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="27"/>
+      <c r="B79" s="27"/>
+      <c r="C79" s="28"/>
+      <c r="D79" s="28"/>
+      <c r="E79" s="32"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="27"/>
+      <c r="B80" s="27"/>
+      <c r="C80" s="28"/>
+      <c r="D80" s="28"/>
+      <c r="E80" s="32"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" s="27"/>
+      <c r="B81" s="27"/>
+      <c r="C81" s="28"/>
+      <c r="D81" s="28"/>
+      <c r="E81" s="32"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A82" s="27"/>
+      <c r="B82" s="27"/>
+      <c r="C82" s="28"/>
+      <c r="D82" s="28"/>
+      <c r="E82" s="32"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A83" s="27"/>
+      <c r="B83" s="27"/>
+      <c r="C83" s="28"/>
+      <c r="D83" s="28"/>
+      <c r="E83" s="32"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A84" s="27"/>
+      <c r="B84" s="27"/>
+      <c r="C84" s="28"/>
+      <c r="D84" s="28"/>
+      <c r="E84" s="32"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A85" s="27"/>
+      <c r="B85" s="27"/>
+      <c r="C85" s="28"/>
+      <c r="D85" s="28"/>
+      <c r="E85" s="32"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A86" s="27"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="28"/>
+      <c r="D86" s="28"/>
+      <c r="E86" s="32"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A87" s="27"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="28"/>
+      <c r="D87" s="28"/>
+      <c r="E87" s="32"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A88" s="27"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="28"/>
+      <c r="D88" s="28"/>
+      <c r="E88" s="32"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A89" s="27"/>
+      <c r="B89" s="27"/>
+      <c r="C89" s="28"/>
+      <c r="D89" s="28"/>
+      <c r="E89" s="32"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A90" s="27"/>
+      <c r="B90" s="27"/>
+      <c r="C90" s="28"/>
+      <c r="D90" s="28"/>
+      <c r="E90" s="32"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A91" s="27"/>
+      <c r="B91" s="27"/>
+      <c r="C91" s="28"/>
+      <c r="D91" s="28"/>
+      <c r="E91" s="32"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A92" s="27"/>
+      <c r="B92" s="27"/>
+      <c r="C92" s="28"/>
+      <c r="D92" s="28"/>
+      <c r="E92" s="32"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A93" s="27"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
+      <c r="D93" s="28"/>
+      <c r="E93" s="32"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A94" s="27"/>
+      <c r="B94" s="27"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="28"/>
+      <c r="E94" s="32"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A95" s="27"/>
+      <c r="B95" s="27"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="32"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A96" s="27"/>
+      <c r="B96" s="27"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="32"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A97" s="27"/>
+      <c r="B97" s="27"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="32"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A98" s="27"/>
+      <c r="B98" s="27"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="32"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A99" s="27"/>
+      <c r="B99" s="27"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="32"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A100" s="27"/>
+      <c r="B100" s="27"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="32"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A101" s="27"/>
+      <c r="B101" s="27"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="32"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A102" s="27"/>
+      <c r="B102" s="27"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="32"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A103" s="27"/>
+      <c r="B103" s="27"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="32"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A104" s="27"/>
+      <c r="B104" s="27"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="32"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A105" s="27"/>
+      <c r="B105" s="27"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="32"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A106" s="27"/>
+      <c r="B106" s="27"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="32"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A107" s="27"/>
+      <c r="B107" s="27"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="32"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A108" s="27"/>
+      <c r="B108" s="27"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="32"/>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A109" s="27"/>
+      <c r="B109" s="27"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="32"/>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A110" s="27"/>
+      <c r="B110" s="27"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="32"/>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A111" s="27"/>
+      <c r="B111" s="27"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="32"/>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A112" s="27"/>
+      <c r="B112" s="27"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="32"/>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A113" s="27"/>
+      <c r="B113" s="27"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="32"/>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A114" s="27"/>
+      <c r="B114" s="27"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="32"/>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" s="27"/>
+      <c r="B115" s="27"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="32"/>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A116" s="27"/>
+      <c r="B116" s="27"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="32"/>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A117" s="27"/>
+      <c r="B117" s="27"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="32"/>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A118" s="27"/>
+      <c r="B118" s="27"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="32"/>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A119" s="27"/>
+      <c r="B119" s="27"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="32"/>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A120" s="27"/>
+      <c r="B120" s="27"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="32"/>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A121" s="27"/>
+      <c r="B121" s="27"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="32"/>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A122" s="27"/>
+      <c r="B122" s="27"/>
+      <c r="C122" s="28"/>
+      <c r="D122" s="28"/>
+      <c r="E122" s="32"/>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A123" s="27"/>
+      <c r="B123" s="27"/>
+      <c r="C123" s="28"/>
+      <c r="D123" s="28"/>
+      <c r="E123" s="32"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A124" s="27"/>
+      <c r="B124" s="27"/>
+      <c r="C124" s="28"/>
+      <c r="D124" s="28"/>
+      <c r="E124" s="32"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A125" s="27"/>
+      <c r="B125" s="27"/>
+      <c r="C125" s="28"/>
+      <c r="D125" s="28"/>
+      <c r="E125" s="32"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A126" s="27"/>
+      <c r="B126" s="27"/>
+      <c r="C126" s="28"/>
+      <c r="D126" s="28"/>
+      <c r="E126" s="32"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A127" s="27"/>
+      <c r="B127" s="27"/>
+      <c r="C127" s="28"/>
+      <c r="D127" s="28"/>
+      <c r="E127" s="32"/>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A128" s="27"/>
+      <c r="B128" s="27"/>
+      <c r="C128" s="28"/>
+      <c r="D128" s="28"/>
+      <c r="E128" s="32"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A129" s="27"/>
+      <c r="B129" s="27"/>
+      <c r="C129" s="28"/>
+      <c r="D129" s="28"/>
+      <c r="E129" s="32"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A130" s="27"/>
+      <c r="B130" s="27"/>
+      <c r="C130" s="28"/>
+      <c r="D130" s="28"/>
+      <c r="E130" s="32"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A131" s="27"/>
+      <c r="B131" s="27"/>
+      <c r="C131" s="28"/>
+      <c r="D131" s="28"/>
+      <c r="E131" s="32"/>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A132" s="27"/>
+      <c r="B132" s="27"/>
+      <c r="C132" s="28"/>
+      <c r="D132" s="28"/>
+      <c r="E132" s="32"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A133" s="27"/>
+      <c r="B133" s="27"/>
+      <c r="C133" s="28"/>
+      <c r="D133" s="28"/>
+      <c r="E133" s="32"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A134" s="27"/>
+      <c r="B134" s="27"/>
+      <c r="C134" s="28"/>
+      <c r="D134" s="28"/>
+      <c r="E134" s="32"/>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A135" s="27"/>
+      <c r="B135" s="27"/>
+      <c r="C135" s="28"/>
+      <c r="D135" s="28"/>
+      <c r="E135" s="32"/>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A136" s="27"/>
+      <c r="B136" s="27"/>
+      <c r="C136" s="28"/>
+      <c r="D136" s="28"/>
+      <c r="E136" s="32"/>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A137" s="27"/>
+      <c r="B137" s="27"/>
+      <c r="C137" s="28"/>
+      <c r="D137" s="28"/>
+      <c r="E137" s="32"/>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A138" s="27"/>
+      <c r="B138" s="27"/>
+      <c r="C138" s="28"/>
+      <c r="D138" s="28"/>
+      <c r="E138" s="32"/>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A139" s="27"/>
+      <c r="B139" s="27"/>
+      <c r="C139" s="28"/>
+      <c r="D139" s="28"/>
+      <c r="E139" s="32"/>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A140" s="27"/>
+      <c r="B140" s="27"/>
+      <c r="C140" s="28"/>
+      <c r="D140" s="28"/>
+      <c r="E140" s="32"/>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A141" s="27"/>
+      <c r="B141" s="27"/>
+      <c r="C141" s="28"/>
+      <c r="D141" s="28"/>
+      <c r="E141" s="32"/>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A142" s="27"/>
+      <c r="B142" s="27"/>
+      <c r="C142" s="28"/>
+      <c r="D142" s="28"/>
+      <c r="E142" s="32"/>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A143" s="27"/>
+      <c r="B143" s="27"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="32"/>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A144" s="27"/>
+      <c r="B144" s="27"/>
+      <c r="C144" s="28"/>
+      <c r="D144" s="28"/>
+      <c r="E144" s="32"/>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A145" s="27"/>
+      <c r="B145" s="27"/>
+      <c r="C145" s="28"/>
+      <c r="D145" s="28"/>
+      <c r="E145" s="32"/>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A146" s="27"/>
+      <c r="B146" s="27"/>
+      <c r="C146" s="28"/>
+      <c r="D146" s="28"/>
+      <c r="E146" s="32"/>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A147" s="27"/>
+      <c r="B147" s="27"/>
+      <c r="C147" s="28"/>
+      <c r="D147" s="28"/>
+      <c r="E147" s="32"/>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A148" s="27"/>
+      <c r="B148" s="27"/>
+      <c r="C148" s="28"/>
+      <c r="D148" s="28"/>
+      <c r="E148" s="32"/>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A149" s="27"/>
+      <c r="B149" s="27"/>
+      <c r="C149" s="28"/>
+      <c r="D149" s="28"/>
+      <c r="E149" s="32"/>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A150" s="27"/>
+      <c r="B150" s="27"/>
+      <c r="C150" s="28"/>
+      <c r="D150" s="28"/>
+      <c r="E150" s="32"/>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A151" s="27"/>
+      <c r="B151" s="27"/>
+      <c r="C151" s="28"/>
+      <c r="D151" s="28"/>
+      <c r="E151" s="32"/>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A152" s="27"/>
+      <c r="B152" s="27"/>
+      <c r="C152" s="28"/>
+      <c r="D152" s="28"/>
+      <c r="E152" s="32"/>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A153" s="27"/>
+      <c r="B153" s="27"/>
+      <c r="C153" s="28"/>
+      <c r="D153" s="28"/>
+      <c r="E153" s="32"/>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A154" s="27"/>
+      <c r="B154" s="27"/>
+      <c r="C154" s="28"/>
+      <c r="D154" s="28"/>
+      <c r="E154" s="32"/>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A155" s="27"/>
+      <c r="B155" s="27"/>
+      <c r="C155" s="28"/>
+      <c r="D155" s="28"/>
+      <c r="E155" s="32"/>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A156" s="27"/>
+      <c r="B156" s="27"/>
+      <c r="C156" s="28"/>
+      <c r="D156" s="28"/>
+      <c r="E156" s="32"/>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A157" s="27"/>
+      <c r="B157" s="27"/>
+      <c r="C157" s="28"/>
+      <c r="D157" s="28"/>
+      <c r="E157" s="32"/>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A158" s="27"/>
+      <c r="B158" s="27"/>
+      <c r="C158" s="28"/>
+      <c r="D158" s="28"/>
+      <c r="E158" s="32"/>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A159" s="27"/>
+      <c r="B159" s="27"/>
+      <c r="C159" s="28"/>
+      <c r="D159" s="28"/>
+      <c r="E159" s="32"/>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A160" s="27"/>
+      <c r="B160" s="27"/>
+      <c r="C160" s="28"/>
+      <c r="D160" s="28"/>
+      <c r="E160" s="32"/>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A161" s="27"/>
+      <c r="B161" s="27"/>
+      <c r="C161" s="28"/>
+      <c r="D161" s="28"/>
+      <c r="E161" s="32"/>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A162" s="27"/>
+      <c r="B162" s="27"/>
+      <c r="C162" s="28"/>
+      <c r="D162" s="28"/>
+      <c r="E162" s="32"/>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A163" s="27"/>
+      <c r="B163" s="27"/>
+      <c r="C163" s="28"/>
+      <c r="D163" s="28"/>
+      <c r="E163" s="32"/>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A164" s="27"/>
+      <c r="B164" s="27"/>
+      <c r="C164" s="28"/>
+      <c r="D164" s="28"/>
+      <c r="E164" s="32"/>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A165" s="27"/>
+      <c r="B165" s="27"/>
+      <c r="C165" s="28"/>
+      <c r="D165" s="28"/>
+      <c r="E165" s="32"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A166" s="27"/>
+      <c r="B166" s="27"/>
+      <c r="C166" s="28"/>
+      <c r="D166" s="28"/>
+      <c r="E166" s="32"/>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A167" s="27"/>
+      <c r="B167" s="27"/>
+      <c r="C167" s="28"/>
+      <c r="D167" s="28"/>
+      <c r="E167" s="32"/>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A168" s="27"/>
+      <c r="B168" s="27"/>
+      <c r="C168" s="28"/>
+      <c r="D168" s="28"/>
+      <c r="E168" s="32"/>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A169" s="27"/>
+      <c r="B169" s="27"/>
+      <c r="C169" s="28"/>
+      <c r="D169" s="28"/>
+      <c r="E169" s="32"/>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A170" s="27"/>
+      <c r="B170" s="27"/>
+      <c r="C170" s="28"/>
+      <c r="D170" s="28"/>
+      <c r="E170" s="32"/>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A171" s="27"/>
+      <c r="B171" s="27"/>
+      <c r="C171" s="28"/>
+      <c r="D171" s="28"/>
+      <c r="E171" s="32"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A172" s="27"/>
+      <c r="B172" s="27"/>
+      <c r="C172" s="28"/>
+      <c r="D172" s="28"/>
+      <c r="E172" s="32"/>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A173" s="27"/>
+      <c r="B173" s="27"/>
+      <c r="C173" s="28"/>
+      <c r="D173" s="28"/>
+      <c r="E173" s="32"/>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A174" s="27"/>
+      <c r="B174" s="27"/>
+      <c r="C174" s="28"/>
+      <c r="D174" s="28"/>
+      <c r="E174" s="32"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A175" s="27"/>
+      <c r="B175" s="27"/>
+      <c r="C175" s="28"/>
+      <c r="D175" s="28"/>
+      <c r="E175" s="32"/>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A176" s="27"/>
+      <c r="B176" s="27"/>
+      <c r="C176" s="28"/>
+      <c r="D176" s="28"/>
+      <c r="E176" s="32"/>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A177" s="27"/>
+      <c r="B177" s="27"/>
+      <c r="C177" s="28"/>
+      <c r="D177" s="28"/>
+      <c r="E177" s="32"/>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A178" s="27"/>
+      <c r="B178" s="27"/>
+      <c r="C178" s="28"/>
+      <c r="D178" s="28"/>
+      <c r="E178" s="32"/>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A179" s="27"/>
+      <c r="B179" s="27"/>
+      <c r="C179" s="28"/>
+      <c r="D179" s="28"/>
+      <c r="E179" s="32"/>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A180" s="27"/>
+      <c r="B180" s="27"/>
+      <c r="C180" s="28"/>
+      <c r="D180" s="28"/>
+      <c r="E180" s="32"/>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A181" s="27"/>
+      <c r="B181" s="27"/>
+      <c r="C181" s="28"/>
+      <c r="D181" s="28"/>
+      <c r="E181" s="32"/>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A182" s="27"/>
+      <c r="B182" s="27"/>
+      <c r="C182" s="28"/>
+      <c r="D182" s="28"/>
+      <c r="E182" s="32"/>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A183" s="27"/>
+      <c r="B183" s="27"/>
+      <c r="C183" s="28"/>
+      <c r="D183" s="28"/>
+      <c r="E183" s="32"/>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A184" s="27"/>
+      <c r="B184" s="27"/>
+      <c r="C184" s="28"/>
+      <c r="D184" s="28"/>
+      <c r="E184" s="32"/>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A185" s="27"/>
+      <c r="B185" s="27"/>
+      <c r="C185" s="28"/>
+      <c r="D185" s="28"/>
+      <c r="E185" s="32"/>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A186" s="27"/>
+      <c r="B186" s="27"/>
+      <c r="C186" s="28"/>
+      <c r="D186" s="28"/>
+      <c r="E186" s="32"/>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A187" s="27"/>
+      <c r="B187" s="27"/>
+      <c r="C187" s="28"/>
+      <c r="D187" s="28"/>
+      <c r="E187" s="32"/>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A188" s="27"/>
+      <c r="B188" s="27"/>
+      <c r="C188" s="28"/>
+      <c r="D188" s="28"/>
+      <c r="E188" s="32"/>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A189" s="27"/>
+      <c r="B189" s="27"/>
+      <c r="C189" s="28"/>
+      <c r="D189" s="28"/>
+      <c r="E189" s="32"/>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A190" s="27"/>
+      <c r="B190" s="27"/>
+      <c r="C190" s="28"/>
+      <c r="D190" s="28"/>
+      <c r="E190" s="32"/>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A191" s="27"/>
+      <c r="B191" s="27"/>
+      <c r="C191" s="28"/>
+      <c r="D191" s="28"/>
+      <c r="E191" s="32"/>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A192" s="27"/>
+      <c r="B192" s="27"/>
+      <c r="C192" s="28"/>
+      <c r="D192" s="28"/>
+      <c r="E192" s="32"/>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A193" s="27"/>
+      <c r="B193" s="27"/>
+      <c r="C193" s="28"/>
+      <c r="D193" s="28"/>
+      <c r="E193" s="32"/>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A194" s="27"/>
+      <c r="B194" s="27"/>
+      <c r="C194" s="28"/>
+      <c r="D194" s="28"/>
+      <c r="E194" s="32"/>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A195" s="27"/>
+      <c r="B195" s="27"/>
+      <c r="C195" s="28"/>
+      <c r="D195" s="28"/>
+      <c r="E195" s="32"/>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A196" s="27"/>
+      <c r="B196" s="27"/>
+      <c r="C196" s="28"/>
+      <c r="D196" s="28"/>
+      <c r="E196" s="32"/>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A197" s="27"/>
+      <c r="B197" s="27"/>
+      <c r="C197" s="28"/>
+      <c r="D197" s="28"/>
+      <c r="E197" s="32"/>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A198" s="27"/>
+      <c r="B198" s="27"/>
+      <c r="C198" s="28"/>
+      <c r="D198" s="28"/>
+      <c r="E198" s="32"/>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A199" s="27"/>
+      <c r="B199" s="27"/>
+      <c r="C199" s="28"/>
+      <c r="D199" s="28"/>
+      <c r="E199" s="32"/>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A200" s="27"/>
+      <c r="B200" s="27"/>
+      <c r="C200" s="28"/>
+      <c r="D200" s="28"/>
+      <c r="E200" s="32"/>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A201" s="33"/>
+      <c r="B201" s="33"/>
+      <c r="C201" s="34"/>
+      <c r="D201" s="34"/>
+      <c r="E201" s="32"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{D8E47E7A-FEC5-43D3-87D4-DDEA82177451}">
+      <formula1>"AllOrNothing,StopOnFirstFailure,ProcessAllIndependently"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>